<commit_message>
added test cases backend for NIH
</commit_message>
<xml_diff>
--- a/DBA(Digital barrier analysis)/TestCase_Import(user and startup).xlsx
+++ b/DBA(Digital barrier analysis)/TestCase_Import(user and startup).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project list" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Safe Job Analysis Page" sheetId="8" r:id="rId6"/>
     <sheet name="Recommendation Page" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -5307,7 +5307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
@@ -15428,7 +15428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I827"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added issue list for dba
</commit_message>
<xml_diff>
--- a/DBA(Digital barrier analysis)/TestCase_Import(user and startup).xlsx
+++ b/DBA(Digital barrier analysis)/TestCase_Import(user and startup).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Project list" sheetId="6" r:id="rId1"/>
@@ -1754,7 +1754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1814,6 +1814,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2096,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,7 +2175,7 @@
       <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -15428,8 +15431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I827"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23985,8 +23988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>